<commit_message>
2 Test cases complete; Passing!
</commit_message>
<xml_diff>
--- a/DeterministicModel/UnitTests/test1-2-excel-calc.xlsx
+++ b/DeterministicModel/UnitTests/test1-2-excel-calc.xlsx
@@ -165,6 +165,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -186,6 +187,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -262,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -299,16 +301,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -323,8 +321,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -410,8 +408,8 @@
   </sheetPr>
   <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S24" activeCellId="0" sqref="S24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,7 +624,7 @@
         <v>3.99920015996801</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
@@ -789,10 +787,10 @@
       <c r="M6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="11" t="n">
+      <c r="N6" s="9" t="n">
         <v>0.136099948898995</v>
       </c>
-      <c r="O6" s="11" t="n">
+      <c r="O6" s="9" t="n">
         <v>0.0199999986666667</v>
       </c>
       <c r="P6" s="8"/>
@@ -851,17 +849,17 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="11" t="n">
         <v>5.632E-005</v>
       </c>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="11" t="n">
         <v>1E-005</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="14" t="n">
+      <c r="G7" s="13" t="n">
         <f aca="false">G5/G6</f>
         <v>0.2</v>
       </c>
@@ -898,15 +896,15 @@
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="11" t="n">
         <v>0.0004301</v>
       </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="11" t="n">
         <v>0.0001</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
       <c r="I8" s="7" t="s">
         <v>22</v>
       </c>
@@ -922,10 +920,10 @@
       <c r="M8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="11" t="n">
+      <c r="N8" s="9" t="n">
         <v>110.793685646268</v>
       </c>
-      <c r="O8" s="11" t="n">
+      <c r="O8" s="9" t="n">
         <v>99.9940003599784</v>
       </c>
       <c r="P8" s="8"/>
@@ -1106,15 +1104,15 @@
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="11" t="n">
         <v>9.248E-005</v>
       </c>
-      <c r="D11" s="12" t="n">
+      <c r="D11" s="11" t="n">
         <v>0.0001</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
       <c r="I11" s="7" t="s">
         <v>25</v>
       </c>
@@ -1187,20 +1185,20 @@
         <v>0.0053665631459995</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="21.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="12" t="n">
+      <c r="C12" s="11" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D12" s="12" t="n">
+      <c r="D12" s="11" t="n">
         <v>0.0001</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
       <c r="I12" s="7" t="s">
         <v>26</v>
       </c>
@@ -1237,36 +1235,36 @@
         <v>26</v>
       </c>
       <c r="V12" s="7" t="n">
-        <f aca="false">1 + SUM(C19:C20)</f>
-        <v>5.00101001</v>
+        <f aca="false">1 +C20</f>
+        <v>5.001</v>
       </c>
       <c r="W12" s="7" t="n">
-        <f aca="false">1 + SUM(D19:D20)</f>
-        <v>5.00001</v>
+        <f aca="false">1 +D20</f>
+        <v>5</v>
       </c>
       <c r="X12" s="8"/>
       <c r="Y12" s="7" t="s">
         <v>26</v>
       </c>
       <c r="Z12" s="7" t="n">
-        <f aca="false">1 + SUM(C19:C21)</f>
-        <v>102.22101001</v>
+        <f aca="false">1 + C21</f>
+        <v>98.22</v>
       </c>
       <c r="AA12" s="7" t="n">
-        <f aca="false">1 + SUM(D19:D21)</f>
-        <v>105.00001</v>
+        <f aca="false">1 + D21</f>
+        <v>101</v>
       </c>
       <c r="AB12" s="8"/>
       <c r="AC12" s="7" t="s">
         <v>26</v>
       </c>
       <c r="AD12" s="7" t="n">
-        <f aca="false">1+SUM(C19:C22)</f>
-        <v>102.23091001</v>
+        <f aca="false">1+C22</f>
+        <v>1.0099</v>
       </c>
       <c r="AE12" s="7" t="n">
-        <f aca="false">1+SUM(D19:D22)</f>
-        <v>105.01001</v>
+        <f aca="false">1+D22</f>
+        <v>1.01</v>
       </c>
       <c r="AF12" s="8"/>
       <c r="AG12" s="7" t="s">
@@ -1277,15 +1275,15 @@
         <v>102.23091001</v>
       </c>
       <c r="AI12" s="7" t="n">
-        <f aca="false">1+SUM(C19:C22)</f>
-        <v>102.23091001</v>
+        <f aca="false">1+SUM(D19:D22)</f>
+        <v>105.01001</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1375,33 +1373,33 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
       <c r="T15" s="8"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
-      <c r="W15" s="9"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
       <c r="X15" s="8"/>
-      <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
+      <c r="Y15" s="14"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
       <c r="AB15" s="8"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
       <c r="AF15" s="8"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
+      <c r="AG15" s="14"/>
+      <c r="AH15" s="14"/>
+      <c r="AI15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -1419,178 +1417,178 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="16" t="n">
+      <c r="J16" s="15" t="n">
         <f aca="false">2 * J3*J4 - 2*J6</f>
         <v>9.64461869547056</v>
       </c>
-      <c r="K16" s="16" t="n">
+      <c r="K16" s="15" t="n">
         <f aca="false">2 * K3*K4 - 2*K6</f>
         <v>7.95840032260268</v>
       </c>
       <c r="L16" s="8"/>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="N16" s="16" t="n">
+      <c r="N16" s="15" t="n">
         <f aca="false">2 * N3*N4 - 2*N6</f>
         <v>9.64461869547056</v>
       </c>
-      <c r="O16" s="16" t="n">
+      <c r="O16" s="15" t="n">
         <f aca="false">2 * O3*O4 - 2*O6</f>
-        <v>7.95840032260268</v>
+        <v>7.95840032260269</v>
       </c>
       <c r="P16" s="8"/>
-      <c r="Q16" s="16" t="s">
+      <c r="Q16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="R16" s="16" t="n">
+      <c r="R16" s="15" t="n">
         <f aca="false">2 * R3*R4 - 2*R6</f>
         <v>9.64461869547056</v>
       </c>
-      <c r="S16" s="16" t="n">
+      <c r="S16" s="15" t="n">
         <f aca="false">2 * S3*S4 - 2*S6</f>
         <v>7.95840032260268</v>
       </c>
       <c r="T16" s="8"/>
-      <c r="U16" s="16" t="s">
+      <c r="U16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="V16" s="16" t="n">
+      <c r="V16" s="15" t="n">
         <f aca="false">2 * V3*V4 - 2*V6</f>
         <v>9.64461869547056</v>
       </c>
-      <c r="W16" s="16" t="n">
+      <c r="W16" s="15" t="n">
         <f aca="false">2 * W3*W4 - 2*W6</f>
         <v>7.95840032260268</v>
       </c>
       <c r="X16" s="8"/>
-      <c r="Y16" s="16" t="s">
+      <c r="Y16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="Z16" s="16" t="n">
+      <c r="Z16" s="15" t="n">
         <f aca="false">2 * Z3*Z4 - 2*Z6</f>
         <v>9.64461869547056</v>
       </c>
-      <c r="AA16" s="16" t="n">
+      <c r="AA16" s="15" t="n">
         <f aca="false">2 * AA3*AA4 - 2*AA6</f>
         <v>7.95840032260268</v>
       </c>
       <c r="AB16" s="8"/>
-      <c r="AC16" s="16" t="s">
+      <c r="AC16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AD16" s="16" t="n">
+      <c r="AD16" s="15" t="n">
         <f aca="false">2 * AD3*AD4 - 2*AD6</f>
         <v>9.64461869547056</v>
       </c>
-      <c r="AE16" s="16" t="n">
+      <c r="AE16" s="15" t="n">
         <f aca="false">2 * AE3*AE4 - 2*AE6</f>
         <v>7.95840032260268</v>
       </c>
       <c r="AF16" s="8"/>
-      <c r="AG16" s="16" t="s">
+      <c r="AG16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AH16" s="16" t="n">
+      <c r="AH16" s="15" t="n">
         <f aca="false">2 * AH3*AH4 - 2*AH6</f>
         <v>-0.27219989779799</v>
       </c>
-      <c r="AI16" s="16" t="n">
+      <c r="AI16" s="15" t="n">
         <f aca="false">2 * AI3*AI4 - 2*AI6</f>
         <v>-0.0399999973333334</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J17" s="16" t="n">
+      <c r="J17" s="15" t="n">
         <f aca="false">-0.5 * J6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="K17" s="16" t="n">
+      <c r="K17" s="15" t="n">
         <f aca="false">-0.5 * K6</f>
         <v>-0.00999999933333335</v>
       </c>
       <c r="L17" s="8"/>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="N17" s="16" t="n">
+      <c r="N17" s="15" t="n">
         <f aca="false">-0.5 * N6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="O17" s="16" t="n">
+      <c r="O17" s="15" t="n">
         <f aca="false">-0.5 * O6</f>
         <v>-0.00999999933333335</v>
       </c>
       <c r="P17" s="8"/>
-      <c r="Q17" s="16" t="s">
+      <c r="Q17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="R17" s="16" t="n">
+      <c r="R17" s="15" t="n">
         <f aca="false">-0.5 * R6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="S17" s="16" t="n">
+      <c r="S17" s="15" t="n">
         <f aca="false">-0.5 * S6</f>
         <v>-0.00999999933333335</v>
       </c>
       <c r="T17" s="8"/>
-      <c r="U17" s="16" t="s">
+      <c r="U17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="V17" s="16" t="n">
+      <c r="V17" s="15" t="n">
         <f aca="false">-0.5 * V6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="W17" s="16" t="n">
+      <c r="W17" s="15" t="n">
         <f aca="false">-0.5 * W6</f>
         <v>-0.00999999933333335</v>
       </c>
       <c r="X17" s="8"/>
-      <c r="Y17" s="16" t="s">
+      <c r="Y17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="Z17" s="16" t="n">
+      <c r="Z17" s="15" t="n">
         <f aca="false">-0.5 * Z6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="AA17" s="16" t="n">
+      <c r="AA17" s="15" t="n">
         <f aca="false">-0.5 * AA6</f>
         <v>-0.00999999933333335</v>
       </c>
       <c r="AB17" s="8"/>
-      <c r="AC17" s="16" t="s">
+      <c r="AC17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AD17" s="16" t="n">
+      <c r="AD17" s="15" t="n">
         <f aca="false">-0.5 * AD6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="AE17" s="16" t="n">
+      <c r="AE17" s="15" t="n">
         <f aca="false">-0.5 * AE6</f>
         <v>-0.00999999933333335</v>
       </c>
       <c r="AF17" s="8"/>
-      <c r="AG17" s="16" t="s">
+      <c r="AG17" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AH17" s="16" t="n">
+      <c r="AH17" s="15" t="n">
         <f aca="false">-0.5 * AH6</f>
         <v>-0.0680499744494974</v>
       </c>
-      <c r="AI17" s="16" t="n">
+      <c r="AI17" s="15" t="n">
         <f aca="false">-0.5 * AI6</f>
         <v>-0.00999999933333335</v>
       </c>
@@ -1611,88 +1609,88 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="16" t="n">
+      <c r="J18" s="15" t="n">
         <f aca="false">-6*J4*J3 - 4 * J6 + J8*J9 + J11*J12</f>
         <v>80.5194376733467</v>
       </c>
-      <c r="K18" s="16" t="n">
+      <c r="K18" s="15" t="n">
         <f aca="false">-6*K4*K3 - 4 * K6 + K8*K9 + K11*K12</f>
         <v>75.9241659686497</v>
       </c>
       <c r="L18" s="8"/>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="N18" s="16" t="n">
+      <c r="N18" s="15" t="n">
         <f aca="false">-6*N4*N3 - 4 * N6 + N8*N9 + N11*N12</f>
         <v>-30.274247972921</v>
       </c>
-      <c r="O18" s="16" t="n">
+      <c r="O18" s="15" t="n">
         <f aca="false">-6*O4*O3 - 4 * O6 + O8*O9 + O11*O12</f>
         <v>-24.0698343913287</v>
       </c>
       <c r="P18" s="8"/>
-      <c r="Q18" s="16" t="s">
+      <c r="Q18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="R18" s="16" t="n">
+      <c r="R18" s="15" t="n">
         <f aca="false">-6*R4*R3 - 4 * R6 + R8*R9 + R11*R12</f>
         <v>-30.2742477666389</v>
       </c>
-      <c r="S18" s="16" t="n">
+      <c r="S18" s="15" t="n">
         <f aca="false">-6*S4*S3 - 4 * S6 + S8*S9 + S11*S12</f>
         <v>-24.0698343376631</v>
       </c>
       <c r="T18" s="8"/>
-      <c r="U18" s="16" t="s">
+      <c r="U18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="V18" s="16" t="n">
+      <c r="V18" s="15" t="n">
         <f aca="false">-6*V4*V3 - 4 * V6 + V8*V9 + V11*V12</f>
-        <v>-30.1917967491139</v>
-      </c>
-      <c r="W18" s="16" t="n">
+        <v>-30.191796955396</v>
+      </c>
+      <c r="W18" s="15" t="n">
         <f aca="false">-6*W4*W3 - 4 * W6 + W8*W9 + W11*W12</f>
-        <v>-24.0483680850791</v>
+        <v>-24.0483681387447</v>
       </c>
       <c r="X18" s="8"/>
-      <c r="Y18" s="16" t="s">
+      <c r="Y18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="Z18" s="16" t="n">
+      <c r="Z18" s="15" t="n">
         <f aca="false">-6*Z4*Z3 - 4 * Z6 + Z8*Z9 + Z11*Z12</f>
-        <v>-28.1883256359462</v>
-      </c>
-      <c r="AA18" s="16" t="n">
+        <v>-28.2707768597534</v>
+      </c>
+      <c r="AA18" s="15" t="n">
         <f aca="false">-6*AA4*AA3 - 4 * AA6 + AA8*AA9 + AA11*AA12</f>
-        <v>-23.5117117704791</v>
+        <v>-23.5331780767288</v>
       </c>
       <c r="AB18" s="8"/>
-      <c r="AC18" s="16" t="s">
+      <c r="AC18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AD18" s="16" t="n">
+      <c r="AD18" s="15" t="n">
         <f aca="false">-6*AD4*AD3 - 4 * AD6 + AD8*AD9 + AD11*AD12</f>
-        <v>-28.1881216206817</v>
-      </c>
-      <c r="AE18" s="16" t="n">
+        <v>-30.2740439576565</v>
+      </c>
+      <c r="AE18" s="15" t="n">
         <f aca="false">-6*AE4*AE3 - 4 * AE6 + AE8*AE9 + AE11*AE12</f>
-        <v>-23.5116581048477</v>
+        <v>-24.0697807256973</v>
       </c>
       <c r="AF18" s="8"/>
-      <c r="AG18" s="16" t="s">
+      <c r="AG18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AH18" s="16" t="n">
+      <c r="AH18" s="15" t="n">
         <f aca="false">-6*AH4*AH3 - 4 * AH6 + AH8*AH9 + AH11*AH12</f>
         <v>1.56233415912398</v>
       </c>
-      <c r="AI18" s="16" t="n">
+      <c r="AI18" s="15" t="n">
         <f aca="false">-6*AI4*AI3 - 4 * AI6 + AI8*AI9 + AI11*AI12</f>
-        <v>0.46862863937499</v>
+        <v>0.483542854960372</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1700,97 +1698,97 @@
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="12" t="n">
+      <c r="C19" s="11" t="n">
         <v>1.001E-005</v>
       </c>
-      <c r="D19" s="12" t="n">
+      <c r="D19" s="11" t="n">
         <v>1E-005</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="I19" s="16" t="s">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="I19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="J19" s="16" t="n">
+      <c r="J19" s="15" t="n">
         <f aca="false">8 * J4*J3 + 2 * J6 - J9*J8 - J12*J11</f>
         <v>-70.8748189778761</v>
       </c>
-      <c r="K19" s="16" t="n">
+      <c r="K19" s="15" t="n">
         <f aca="false">8 * K4*K3 + 2 * K6 - K9*K8 - K12*K11</f>
         <v>-67.965765646047</v>
       </c>
       <c r="L19" s="8"/>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="16" t="n">
+      <c r="N19" s="15" t="n">
         <f aca="false">8 * N4*N3 + 2 * N6 - N9*N8 - N12*N11</f>
         <v>39.9188666683916</v>
       </c>
-      <c r="O19" s="16" t="n">
+      <c r="O19" s="15" t="n">
         <f aca="false">8 * O4*O3 + 2 * O6 - O9*O8 - O12*O11</f>
         <v>32.0282347139314</v>
       </c>
       <c r="P19" s="8"/>
-      <c r="Q19" s="16" t="s">
+      <c r="Q19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="R19" s="16" t="n">
+      <c r="R19" s="15" t="n">
         <f aca="false">8 * R4*R3 + 2 * R6 - R9*R8 - R12*R11</f>
         <v>39.9188664621095</v>
       </c>
-      <c r="S19" s="16" t="n">
+      <c r="S19" s="15" t="n">
         <f aca="false">8 * S4*S3 + 2 * S6 - S9*S8 - S12*S11</f>
         <v>32.0282346602658</v>
       </c>
       <c r="T19" s="8"/>
-      <c r="U19" s="16" t="s">
+      <c r="U19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="V19" s="16" t="n">
+      <c r="V19" s="15" t="n">
         <f aca="false">8 * V4*V3 + 2 * V6 - V9*V8 - V12*V11</f>
-        <v>39.8364154445844</v>
-      </c>
-      <c r="W19" s="16" t="n">
+        <v>39.8364156508666</v>
+      </c>
+      <c r="W19" s="15" t="n">
         <f aca="false">8 * W4*W3 + 2 * W6 - W9*W8 - W12*W11</f>
-        <v>32.0067684076818</v>
+        <v>32.0067684613474</v>
       </c>
       <c r="X19" s="8"/>
-      <c r="Y19" s="16" t="s">
+      <c r="Y19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="Z19" s="16" t="n">
+      <c r="Z19" s="15" t="n">
         <f aca="false">8 * Z4*Z3 + 2 * Z6 - Z9*Z8 - Z12*Z11</f>
-        <v>37.8329443314168</v>
-      </c>
-      <c r="AA19" s="16" t="n">
+        <v>37.915395555224</v>
+      </c>
+      <c r="AA19" s="15" t="n">
         <f aca="false">8 * AA4*AA3 + 2 * AA6 - AA9*AA8 - AA12*AA11</f>
-        <v>31.4701120930818</v>
+        <v>31.4915783993315</v>
       </c>
       <c r="AB19" s="8"/>
-      <c r="AC19" s="16" t="s">
+      <c r="AC19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AD19" s="16" t="n">
+      <c r="AD19" s="15" t="n">
         <f aca="false">8 * AD4*AD3 + 2 * AD6 - AD9*AD8 - AD12*AD11</f>
-        <v>37.8327403161522</v>
-      </c>
-      <c r="AE19" s="16" t="n">
+        <v>39.918662653127</v>
+      </c>
+      <c r="AE19" s="15" t="n">
         <f aca="false">8 * AE4*AE3 + 2 * AE6 - AE9*AE8 - AE12*AE11</f>
-        <v>31.4700584274504</v>
+        <v>32.0281810483</v>
       </c>
       <c r="AF19" s="8"/>
-      <c r="AG19" s="16" t="s">
+      <c r="AG19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AH19" s="16" t="n">
+      <c r="AH19" s="15" t="n">
         <f aca="false">8 * AH4*AH3 + 2 * AH6 - AH9*AH8 - AH12*AH11</f>
         <v>-1.83453405692197</v>
       </c>
-      <c r="AI19" s="16" t="n">
+      <c r="AI19" s="15" t="n">
         <f aca="false">8 * AI4*AI3 + 2 * AI6 - AI9*AI8 - AI12*AI11</f>
-        <v>-0.508628636708324</v>
+        <v>-0.523542852293706</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,15 +1852,15 @@
       <c r="B24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="12" t="n">
+      <c r="C24" s="11" t="n">
         <v>1.115E-006</v>
       </c>
-      <c r="D24" s="12" t="n">
+      <c r="D24" s="11" t="n">
         <v>1E-006</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Add fit image; add top solutions collage image
</commit_message>
<xml_diff>
--- a/DeterministicModel/UnitTests/test1-2-excel-calc.xlsx
+++ b/DeterministicModel/UnitTests/test1-2-excel-calc.xlsx
@@ -408,8 +408,8 @@
   </sheetPr>
   <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>